<commit_message>
add optional email to feedback page add email to body of email make sure that email is only being send once when send is pressed
</commit_message>
<xml_diff>
--- a/Assets/Editor/RFScenarios/Groningen/AllGroningenScenariosEnglish.xlsx
+++ b/Assets/Editor/RFScenarios/Groningen/AllGroningenScenariosEnglish.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\INSPEC2T\ResourceForce\RF_Game\Assets\Resources\RFScenarios\Groningen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\INSPEC2T\ResourceForce\RF_Game\Assets\Editor\RFScenarios\Groningen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>There is a whole trail of vandalism. Students are even walking on rooftops of cars.</t>
-  </si>
-  <si>
-    <t>A citizen sends a picture showing three people molesting bicycles</t>
   </si>
   <si>
     <t>Unfortunately, the perpetrators can not be traced and arrested.</t>
@@ -696,6 +693,9 @@
   <si>
     <t>112 is called and an ambulance is on its way.</t>
   </si>
+  <si>
+    <t>A citizen sends a picture showing three people vandalising bicycles</t>
+  </si>
 </sst>
 </file>
 
@@ -871,14 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -888,6 +880,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1189,9 +1189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M83" sqref="M83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1203,30 +1203,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="12" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1"/>
@@ -1247,10 +1247,10 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1260,9 +1260,9 @@
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1301,10 +1301,10 @@
       <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="7">
@@ -1331,20 +1331,20 @@
       <c r="L3" s="7">
         <v>3</v>
       </c>
-      <c r="M3" s="13" t="s">
-        <v>158</v>
+      <c r="M3" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="N3" s="7">
         <v>3</v>
       </c>
-      <c r="O3" s="13" t="s">
-        <v>159</v>
+      <c r="O3" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="P3" s="7">
         <v>4</v>
       </c>
-      <c r="Q3" s="13" t="s">
-        <v>160</v>
+      <c r="Q3" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -1363,10 +1363,10 @@
       <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="7">
@@ -1393,20 +1393,20 @@
       <c r="L4" s="7">
         <v>3</v>
       </c>
-      <c r="M4" s="13" t="s">
-        <v>161</v>
+      <c r="M4" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="N4" s="7">
         <v>4</v>
       </c>
-      <c r="O4" s="13" t="s">
-        <v>162</v>
+      <c r="O4" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="P4" s="7">
         <v>4</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>163</v>
+      <c r="Q4" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -1425,10 +1425,10 @@
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="7">
@@ -1455,20 +1455,20 @@
       <c r="L5" s="7">
         <v>1</v>
       </c>
-      <c r="M5" s="13" t="s">
-        <v>164</v>
+      <c r="M5" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="N5" s="7">
         <v>3</v>
       </c>
-      <c r="O5" s="13" t="s">
-        <v>165</v>
+      <c r="O5" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="P5" s="7">
         <v>2</v>
       </c>
-      <c r="Q5" s="13" t="s">
-        <v>166</v>
+      <c r="Q5" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -1487,10 +1487,10 @@
       <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="7">
@@ -1517,8 +1517,8 @@
       <c r="L6" s="7">
         <v>3</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>167</v>
+      <c r="M6" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="N6" s="7">
         <v>-1</v>
@@ -1549,10 +1549,10 @@
       <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="7">
@@ -1579,14 +1579,14 @@
       <c r="L7" s="7">
         <v>2</v>
       </c>
-      <c r="M7" s="13" t="s">
-        <v>168</v>
+      <c r="M7" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="N7" s="7">
         <v>4</v>
       </c>
-      <c r="O7" s="13" t="s">
-        <v>169</v>
+      <c r="O7" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="P7" s="7">
         <v>-1</v>
@@ -1612,9 +1612,9 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="7">
@@ -1674,9 +1674,9 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="7">
@@ -1736,9 +1736,9 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="7">
@@ -1798,9 +1798,9 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="7">
@@ -1859,10 +1859,10 @@
       <c r="B12" s="7">
         <v>1</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="7">
@@ -1889,20 +1889,20 @@
       <c r="L12" s="7">
         <v>1</v>
       </c>
-      <c r="M12" s="13" t="s">
-        <v>170</v>
+      <c r="M12" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="N12" s="7">
         <v>3</v>
       </c>
-      <c r="O12" s="13" t="s">
-        <v>171</v>
+      <c r="O12" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P12" s="7">
         <v>4</v>
       </c>
-      <c r="Q12" s="13" t="s">
-        <v>172</v>
+      <c r="Q12" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
@@ -1921,10 +1921,10 @@
       <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="7">
@@ -1951,20 +1951,20 @@
       <c r="L13" s="7">
         <v>1</v>
       </c>
-      <c r="M13" s="13" t="s">
-        <v>170</v>
+      <c r="M13" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="N13" s="7">
         <v>3</v>
       </c>
-      <c r="O13" s="13" t="s">
-        <v>173</v>
+      <c r="O13" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="P13" s="7">
         <v>4</v>
       </c>
-      <c r="Q13" s="13" t="s">
-        <v>174</v>
+      <c r="Q13" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
@@ -1983,10 +1983,10 @@
       <c r="B14" s="7">
         <v>3</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="7">
@@ -2013,8 +2013,8 @@
       <c r="L14" s="7">
         <v>3</v>
       </c>
-      <c r="M14" s="13" t="s">
-        <v>175</v>
+      <c r="M14" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="N14" s="7">
         <v>-1</v>
@@ -2045,10 +2045,10 @@
       <c r="B15" s="7">
         <v>4</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="7">
@@ -2075,8 +2075,8 @@
       <c r="L15" s="7">
         <v>4</v>
       </c>
-      <c r="M15" s="13" t="s">
-        <v>176</v>
+      <c r="M15" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="N15" s="7">
         <v>-1</v>
@@ -2107,10 +2107,10 @@
       <c r="B16" s="7">
         <v>5</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="7">
@@ -2137,8 +2137,8 @@
       <c r="L16" s="7">
         <v>4</v>
       </c>
-      <c r="M16" s="13" t="s">
-        <v>177</v>
+      <c r="M16" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="N16" s="7">
         <v>-1</v>
@@ -2170,9 +2170,9 @@
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="7">
@@ -2232,9 +2232,9 @@
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="7">
@@ -2294,9 +2294,9 @@
         <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="7">
@@ -2356,9 +2356,9 @@
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="7">
@@ -2417,10 +2417,10 @@
       <c r="B21" s="7">
         <v>1</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="7">
@@ -2447,20 +2447,20 @@
       <c r="L21" s="7">
         <v>3</v>
       </c>
-      <c r="M21" s="13" t="s">
-        <v>178</v>
+      <c r="M21" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="N21" s="7">
         <v>3</v>
       </c>
-      <c r="O21" s="13" t="s">
-        <v>171</v>
+      <c r="O21" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P21" s="7">
         <v>4</v>
       </c>
-      <c r="Q21" s="13" t="s">
-        <v>179</v>
+      <c r="Q21" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -2479,10 +2479,10 @@
       <c r="B22" s="7">
         <v>2</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="13" t="s">
+      <c r="C22" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="7">
@@ -2509,20 +2509,20 @@
       <c r="L22" s="7">
         <v>2</v>
       </c>
-      <c r="M22" s="13" t="s">
-        <v>180</v>
+      <c r="M22" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="N22" s="7">
         <v>4</v>
       </c>
-      <c r="O22" s="13" t="s">
-        <v>181</v>
+      <c r="O22" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="P22" s="7">
         <v>2</v>
       </c>
-      <c r="Q22" s="13" t="s">
-        <v>166</v>
+      <c r="Q22" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -2541,10 +2541,10 @@
       <c r="B23" s="7">
         <v>3</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="C23" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="7">
@@ -2571,20 +2571,20 @@
       <c r="L23" s="7">
         <v>3</v>
       </c>
-      <c r="M23" s="13" t="s">
-        <v>178</v>
+      <c r="M23" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="N23" s="7">
         <v>3</v>
       </c>
-      <c r="O23" s="13" t="s">
-        <v>171</v>
+      <c r="O23" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P23" s="7">
         <v>4</v>
       </c>
-      <c r="Q23" s="13" t="s">
-        <v>179</v>
+      <c r="Q23" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
@@ -2603,10 +2603,10 @@
       <c r="B24" s="7">
         <v>4</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="7">
@@ -2633,14 +2633,14 @@
       <c r="L24" s="7">
         <v>2</v>
       </c>
-      <c r="M24" s="13" t="s">
-        <v>180</v>
+      <c r="M24" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="N24" s="7">
         <v>4</v>
       </c>
-      <c r="O24" s="13" t="s">
-        <v>169</v>
+      <c r="O24" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="P24" s="7">
         <v>-1</v>
@@ -2666,9 +2666,9 @@
         <v>5</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="7">
@@ -2728,9 +2728,9 @@
         <v>6</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="7">
@@ -2790,9 +2790,9 @@
         <v>7</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E27" s="7">
@@ -2851,10 +2851,10 @@
       <c r="B28" s="7">
         <v>1</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" s="13" t="s">
+      <c r="C28" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="7">
@@ -2881,20 +2881,20 @@
       <c r="L28" s="7">
         <v>3</v>
       </c>
-      <c r="M28" s="13" t="s">
-        <v>182</v>
+      <c r="M28" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="N28" s="7">
         <v>3</v>
       </c>
-      <c r="O28" s="13" t="s">
-        <v>183</v>
+      <c r="O28" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="P28" s="7">
         <v>4</v>
       </c>
-      <c r="Q28" s="13" t="s">
-        <v>184</v>
+      <c r="Q28" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
@@ -2913,10 +2913,10 @@
       <c r="B29" s="7">
         <v>2</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="13" t="s">
+      <c r="C29" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E29" s="7">
@@ -2943,8 +2943,8 @@
       <c r="L29" s="7">
         <v>3</v>
       </c>
-      <c r="M29" s="13" t="s">
-        <v>182</v>
+      <c r="M29" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="N29" s="7">
         <v>-1</v>
@@ -2955,8 +2955,8 @@
       <c r="P29" s="7">
         <v>4</v>
       </c>
-      <c r="Q29" s="13" t="s">
-        <v>184</v>
+      <c r="Q29" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
@@ -2975,10 +2975,10 @@
       <c r="B30" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="13" t="s">
+      <c r="C30" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="7">
@@ -3005,20 +3005,20 @@
       <c r="L30" s="7">
         <v>1</v>
       </c>
-      <c r="M30" s="13" t="s">
-        <v>185</v>
+      <c r="M30" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="N30" s="7">
         <v>3</v>
       </c>
-      <c r="O30" s="13" t="s">
-        <v>186</v>
+      <c r="O30" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="P30" s="7">
         <v>4</v>
       </c>
-      <c r="Q30" s="13" t="s">
-        <v>184</v>
+      <c r="Q30" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
@@ -3037,10 +3037,10 @@
       <c r="B31" s="7">
         <v>4</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="13" t="s">
+      <c r="C31" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="7">
@@ -3067,14 +3067,14 @@
       <c r="L31" s="7">
         <v>1</v>
       </c>
-      <c r="M31" s="13" t="s">
-        <v>185</v>
+      <c r="M31" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="N31" s="7">
         <v>3</v>
       </c>
-      <c r="O31" s="13" t="s">
-        <v>186</v>
+      <c r="O31" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="P31" s="7">
         <v>-1</v>
@@ -3100,9 +3100,9 @@
         <v>5</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E32" s="7">
@@ -3162,9 +3162,9 @@
         <v>6</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="7">
@@ -3223,10 +3223,10 @@
       <c r="B34" s="7">
         <v>1</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="13" t="s">
+      <c r="C34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>59</v>
       </c>
       <c r="E34" s="7">
@@ -3253,20 +3253,20 @@
       <c r="L34" s="7">
         <v>2</v>
       </c>
-      <c r="M34" s="13" t="s">
-        <v>178</v>
+      <c r="M34" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="N34" s="7">
         <v>3</v>
       </c>
-      <c r="O34" s="13" t="s">
-        <v>171</v>
+      <c r="O34" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P34" s="7">
         <v>4</v>
       </c>
-      <c r="Q34" s="13" t="s">
-        <v>187</v>
+      <c r="Q34" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="R34" s="6"/>
       <c r="S34" s="6"/>
@@ -3285,10 +3285,10 @@
       <c r="B35" s="7">
         <v>2</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D35" s="13" t="s">
+      <c r="C35" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E35" s="7">
@@ -3315,20 +3315,20 @@
       <c r="L35" s="7">
         <v>2</v>
       </c>
-      <c r="M35" s="13" t="s">
-        <v>161</v>
+      <c r="M35" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="N35" s="7">
         <v>3</v>
       </c>
-      <c r="O35" s="13" t="s">
-        <v>188</v>
+      <c r="O35" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="P35" s="7">
         <v>2</v>
       </c>
-      <c r="Q35" s="13" t="s">
-        <v>166</v>
+      <c r="Q35" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
@@ -3347,11 +3347,11 @@
       <c r="B36" s="7">
         <v>3</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>61</v>
+      <c r="C36" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>224</v>
       </c>
       <c r="E36" s="7">
         <v>4</v>
@@ -3377,14 +3377,14 @@
       <c r="L36" s="7">
         <v>1</v>
       </c>
-      <c r="M36" s="13" t="s">
-        <v>189</v>
+      <c r="M36" s="9" t="s">
+        <v>188</v>
       </c>
       <c r="N36" s="7">
         <v>4</v>
       </c>
-      <c r="O36" s="13" t="s">
-        <v>169</v>
+      <c r="O36" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="P36" s="7">
         <v>-1</v>
@@ -3410,10 +3410,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>62</v>
+        <v>112</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="E37" s="7">
         <v>-1</v>
@@ -3472,10 +3472,10 @@
         <v>5</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>63</v>
+        <v>112</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="E38" s="7">
         <v>-1</v>
@@ -3533,11 +3533,11 @@
       <c r="B39" s="7">
         <v>1</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>64</v>
+      <c r="C39" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="E39" s="7">
         <v>2</v>
@@ -3563,20 +3563,20 @@
       <c r="L39" s="7">
         <v>3</v>
       </c>
-      <c r="M39" s="13" t="s">
-        <v>190</v>
+      <c r="M39" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="N39" s="7">
         <v>3</v>
       </c>
-      <c r="O39" s="13" t="s">
-        <v>183</v>
+      <c r="O39" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="P39" s="7">
         <v>3</v>
       </c>
-      <c r="Q39" s="13" t="s">
-        <v>191</v>
+      <c r="Q39" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
@@ -3595,11 +3595,11 @@
       <c r="B40" s="7">
         <v>2</v>
       </c>
-      <c r="C40" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>65</v>
+      <c r="C40" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="E40" s="7">
         <v>4</v>
@@ -3625,20 +3625,20 @@
       <c r="L40" s="7">
         <v>2</v>
       </c>
-      <c r="M40" s="13" t="s">
-        <v>192</v>
+      <c r="M40" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="N40" s="7">
         <v>3</v>
       </c>
-      <c r="O40" s="13" t="s">
-        <v>183</v>
+      <c r="O40" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="P40" s="7">
         <v>3</v>
       </c>
-      <c r="Q40" s="13" t="s">
-        <v>191</v>
+      <c r="Q40" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="R40" s="6"/>
       <c r="S40" s="6"/>
@@ -3657,11 +3657,11 @@
       <c r="B41" s="7">
         <v>3</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>66</v>
+      <c r="C41" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E41" s="7">
         <v>7</v>
@@ -3687,8 +3687,8 @@
       <c r="L41" s="7">
         <v>2</v>
       </c>
-      <c r="M41" s="13" t="s">
-        <v>193</v>
+      <c r="M41" s="9" t="s">
+        <v>192</v>
       </c>
       <c r="N41" s="7">
         <v>-1</v>
@@ -3699,8 +3699,8 @@
       <c r="P41" s="7">
         <v>3</v>
       </c>
-      <c r="Q41" s="13" t="s">
-        <v>191</v>
+      <c r="Q41" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="R41" s="6"/>
       <c r="S41" s="6"/>
@@ -3719,11 +3719,11 @@
       <c r="B42" s="7">
         <v>4</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>67</v>
+      <c r="C42" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="E42" s="7">
         <v>7</v>
@@ -3749,20 +3749,20 @@
       <c r="L42" s="7">
         <v>2</v>
       </c>
-      <c r="M42" s="13" t="s">
-        <v>194</v>
+      <c r="M42" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="N42" s="7">
         <v>3</v>
       </c>
-      <c r="O42" s="13" t="s">
-        <v>171</v>
+      <c r="O42" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P42" s="7">
         <v>3</v>
       </c>
-      <c r="Q42" s="13" t="s">
-        <v>191</v>
+      <c r="Q42" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="R42" s="6"/>
       <c r="S42" s="6"/>
@@ -3781,11 +3781,11 @@
       <c r="B43" s="7">
         <v>5</v>
       </c>
-      <c r="C43" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>68</v>
+      <c r="C43" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="E43" s="7">
         <v>7</v>
@@ -3811,14 +3811,14 @@
       <c r="L43" s="7">
         <v>2</v>
       </c>
-      <c r="M43" s="13" t="s">
-        <v>194</v>
+      <c r="M43" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="N43" s="7">
         <v>4</v>
       </c>
-      <c r="O43" s="13" t="s">
-        <v>169</v>
+      <c r="O43" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="P43" s="7">
         <v>-1</v>
@@ -3844,10 +3844,10 @@
         <v>6</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>69</v>
+        <v>112</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E44" s="7">
         <v>-1</v>
@@ -3905,11 +3905,11 @@
       <c r="B45" s="7">
         <v>7</v>
       </c>
-      <c r="C45" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>70</v>
+      <c r="C45" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="E45" s="7">
         <v>-1</v>
@@ -3967,11 +3967,11 @@
       <c r="B46" s="7">
         <v>1</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>71</v>
+      <c r="C46" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="E46" s="7">
         <v>2</v>
@@ -3997,20 +3997,20 @@
       <c r="L46" s="7">
         <v>3</v>
       </c>
-      <c r="M46" s="13" t="s">
-        <v>195</v>
+      <c r="M46" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="N46" s="7">
         <v>3</v>
       </c>
-      <c r="O46" s="13" t="s">
-        <v>171</v>
+      <c r="O46" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P46" s="7">
         <v>4</v>
       </c>
-      <c r="Q46" s="13" t="s">
-        <v>196</v>
+      <c r="Q46" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="R46" s="6"/>
       <c r="S46" s="6"/>
@@ -4029,11 +4029,11 @@
       <c r="B47" s="7">
         <v>2</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>72</v>
+      <c r="C47" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="E47" s="7">
         <v>4</v>
@@ -4059,20 +4059,20 @@
       <c r="L47" s="7">
         <v>2</v>
       </c>
-      <c r="M47" s="13" t="s">
-        <v>192</v>
+      <c r="M47" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="N47" s="7">
         <v>3</v>
       </c>
-      <c r="O47" s="13" t="s">
-        <v>171</v>
+      <c r="O47" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="P47" s="7">
         <v>4</v>
       </c>
-      <c r="Q47" s="13" t="s">
-        <v>196</v>
+      <c r="Q47" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="R47" s="6"/>
       <c r="S47" s="6"/>
@@ -4091,11 +4091,11 @@
       <c r="B48" s="7">
         <v>3</v>
       </c>
-      <c r="C48" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>73</v>
+      <c r="C48" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="E48" s="7">
         <v>5</v>
@@ -4121,8 +4121,8 @@
       <c r="L48" s="7">
         <v>3</v>
       </c>
-      <c r="M48" s="13" t="s">
-        <v>197</v>
+      <c r="M48" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="N48" s="7">
         <v>-1</v>
@@ -4153,11 +4153,11 @@
       <c r="B49" s="7">
         <v>4</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>74</v>
+      <c r="C49" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="E49" s="7">
         <v>5</v>
@@ -4183,14 +4183,14 @@
       <c r="L49" s="7">
         <v>2</v>
       </c>
-      <c r="M49" s="13" t="s">
-        <v>198</v>
+      <c r="M49" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N49" s="7">
         <v>3</v>
       </c>
-      <c r="O49" s="13" t="s">
-        <v>183</v>
+      <c r="O49" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="P49" s="7">
         <v>-1</v>
@@ -4215,11 +4215,11 @@
       <c r="B50" s="7">
         <v>5</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>75</v>
+      <c r="C50" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E50" s="7">
         <v>10</v>
@@ -4245,14 +4245,14 @@
       <c r="L50" s="7">
         <v>1</v>
       </c>
-      <c r="M50" s="13" t="s">
-        <v>199</v>
+      <c r="M50" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="N50" s="7">
         <v>4</v>
       </c>
-      <c r="O50" s="13" t="s">
-        <v>188</v>
+      <c r="O50" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="P50" s="7">
         <v>-1</v>
@@ -4277,11 +4277,11 @@
       <c r="B51" s="7">
         <v>6</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>76</v>
+      <c r="C51" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E51" s="7">
         <v>10</v>
@@ -4307,20 +4307,20 @@
       <c r="L51" s="7">
         <v>1</v>
       </c>
-      <c r="M51" s="13" t="s">
-        <v>199</v>
+      <c r="M51" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="N51" s="7">
         <v>3</v>
       </c>
-      <c r="O51" s="13" t="s">
-        <v>200</v>
+      <c r="O51" s="9" t="s">
+        <v>199</v>
       </c>
       <c r="P51" s="7">
         <v>4</v>
       </c>
-      <c r="Q51" s="13" t="s">
-        <v>201</v>
+      <c r="Q51" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="R51" s="6"/>
       <c r="S51" s="6"/>
@@ -4339,11 +4339,11 @@
       <c r="B52" s="7">
         <v>7</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>77</v>
+      <c r="C52" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="E52" s="7">
         <v>10</v>
@@ -4369,20 +4369,20 @@
       <c r="L52" s="7">
         <v>1</v>
       </c>
-      <c r="M52" s="13" t="s">
-        <v>199</v>
+      <c r="M52" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="N52" s="7">
         <v>3</v>
       </c>
-      <c r="O52" s="13" t="s">
-        <v>202</v>
+      <c r="O52" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="P52" s="7">
         <v>4</v>
       </c>
-      <c r="Q52" s="13" t="s">
-        <v>201</v>
+      <c r="Q52" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="R52" s="6"/>
       <c r="S52" s="6"/>
@@ -4401,11 +4401,11 @@
       <c r="B53" s="7">
         <v>8</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>78</v>
+      <c r="C53" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="E53" s="7">
         <v>10</v>
@@ -4431,14 +4431,14 @@
       <c r="L53" s="7">
         <v>1</v>
       </c>
-      <c r="M53" s="13" t="s">
-        <v>199</v>
+      <c r="M53" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="N53" s="7">
         <v>4</v>
       </c>
-      <c r="O53" s="13" t="s">
-        <v>169</v>
+      <c r="O53" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="P53" s="7">
         <v>-1</v>
@@ -4463,11 +4463,11 @@
       <c r="B54" s="7">
         <v>9</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>79</v>
+      <c r="C54" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="E54" s="7">
         <v>10</v>
@@ -4493,8 +4493,8 @@
       <c r="L54" s="7">
         <v>1</v>
       </c>
-      <c r="M54" s="13" t="s">
-        <v>203</v>
+      <c r="M54" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="N54" s="7">
         <v>-1</v>
@@ -4505,8 +4505,8 @@
       <c r="P54" s="7">
         <v>4</v>
       </c>
-      <c r="Q54" s="13" t="s">
-        <v>204</v>
+      <c r="Q54" s="9" t="s">
+        <v>203</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
@@ -4526,10 +4526,10 @@
         <v>10</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>80</v>
+        <v>112</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E55" s="7">
         <v>-1</v>
@@ -4588,10 +4588,10 @@
         <v>11</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>81</v>
+        <v>112</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="E56" s="7">
         <v>-1</v>
@@ -4649,11 +4649,11 @@
       <c r="B57" s="7">
         <v>1</v>
       </c>
-      <c r="C57" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>82</v>
+      <c r="C57" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="E57" s="7">
         <v>3</v>
@@ -4679,20 +4679,20 @@
       <c r="L57" s="7">
         <v>3</v>
       </c>
-      <c r="M57" s="13" t="s">
-        <v>195</v>
+      <c r="M57" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="N57" s="7">
         <v>3</v>
       </c>
-      <c r="O57" s="13" t="s">
-        <v>205</v>
+      <c r="O57" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="P57" s="7">
         <v>3</v>
       </c>
-      <c r="Q57" s="13" t="s">
-        <v>206</v>
+      <c r="Q57" s="9" t="s">
+        <v>205</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
@@ -4711,11 +4711,11 @@
       <c r="B58" s="7">
         <v>2</v>
       </c>
-      <c r="C58" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>83</v>
+      <c r="C58" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="E58" s="7">
         <v>3</v>
@@ -4741,20 +4741,20 @@
       <c r="L58" s="7">
         <v>1</v>
       </c>
-      <c r="M58" s="13" t="s">
-        <v>207</v>
+      <c r="M58" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="N58" s="7">
         <v>4</v>
       </c>
-      <c r="O58" s="13" t="s">
-        <v>188</v>
+      <c r="O58" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="P58" s="7">
         <v>3</v>
       </c>
-      <c r="Q58" s="13" t="s">
-        <v>206</v>
+      <c r="Q58" s="9" t="s">
+        <v>205</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -4773,11 +4773,11 @@
       <c r="B59" s="7">
         <v>3</v>
       </c>
-      <c r="C59" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>84</v>
+      <c r="C59" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="E59" s="7">
         <v>4</v>
@@ -4803,20 +4803,20 @@
       <c r="L59" s="7">
         <v>1</v>
       </c>
-      <c r="M59" s="13" t="s">
-        <v>208</v>
+      <c r="M59" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="N59" s="7">
         <v>4</v>
       </c>
-      <c r="O59" s="13" t="s">
-        <v>188</v>
+      <c r="O59" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="P59" s="7">
         <v>2</v>
       </c>
-      <c r="Q59" s="13" t="s">
-        <v>209</v>
+      <c r="Q59" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -4835,11 +4835,11 @@
       <c r="B60" s="7">
         <v>4</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>85</v>
+      <c r="C60" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="E60" s="7">
         <v>5</v>
@@ -4865,20 +4865,20 @@
       <c r="L60" s="7">
         <v>1</v>
       </c>
-      <c r="M60" s="13" t="s">
-        <v>210</v>
+      <c r="M60" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="N60" s="7">
         <v>3</v>
       </c>
-      <c r="O60" s="13" t="s">
-        <v>211</v>
+      <c r="O60" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="P60" s="7">
         <v>2</v>
       </c>
-      <c r="Q60" s="13" t="s">
-        <v>209</v>
+      <c r="Q60" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
@@ -4897,11 +4897,11 @@
       <c r="B61" s="7">
         <v>5</v>
       </c>
-      <c r="C61" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>86</v>
+      <c r="C61" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="E61" s="7">
         <v>9</v>
@@ -4927,14 +4927,14 @@
       <c r="L61" s="7">
         <v>1</v>
       </c>
-      <c r="M61" s="13" t="s">
-        <v>212</v>
+      <c r="M61" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="N61" s="7">
         <v>3</v>
       </c>
-      <c r="O61" s="13" t="s">
-        <v>213</v>
+      <c r="O61" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="P61" s="7">
         <v>-1</v>
@@ -4959,11 +4959,11 @@
       <c r="B62" s="7">
         <v>6</v>
       </c>
-      <c r="C62" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>87</v>
+      <c r="C62" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="E62" s="7">
         <v>10</v>
@@ -4989,8 +4989,8 @@
       <c r="L62" s="7">
         <v>3</v>
       </c>
-      <c r="M62" s="13" t="s">
-        <v>214</v>
+      <c r="M62" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="N62" s="7">
         <v>-1</v>
@@ -5021,11 +5021,11 @@
       <c r="B63" s="7">
         <v>7</v>
       </c>
-      <c r="C63" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>88</v>
+      <c r="C63" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="E63" s="7">
         <v>8</v>
@@ -5051,8 +5051,8 @@
       <c r="L63" s="7">
         <v>3</v>
       </c>
-      <c r="M63" s="13" t="s">
-        <v>215</v>
+      <c r="M63" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="N63" s="7">
         <v>-1</v>
@@ -5083,11 +5083,11 @@
       <c r="B64" s="7">
         <v>8</v>
       </c>
-      <c r="C64" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>89</v>
+      <c r="C64" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="E64" s="7">
         <v>11</v>
@@ -5113,8 +5113,8 @@
       <c r="L64" s="7">
         <v>2</v>
       </c>
-      <c r="M64" s="13" t="s">
-        <v>198</v>
+      <c r="M64" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N64" s="7">
         <v>-1</v>
@@ -5125,8 +5125,8 @@
       <c r="P64" s="7">
         <v>4</v>
       </c>
-      <c r="Q64" s="13" t="s">
-        <v>216</v>
+      <c r="Q64" s="9" t="s">
+        <v>215</v>
       </c>
       <c r="R64" s="2"/>
       <c r="S64" s="2"/>
@@ -5146,10 +5146,10 @@
         <v>9</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>90</v>
+        <v>112</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="E65" s="7">
         <v>-1</v>
@@ -5208,10 +5208,10 @@
         <v>10</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>91</v>
+        <v>112</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="E66" s="7">
         <v>-1</v>
@@ -5270,10 +5270,10 @@
         <v>11</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>92</v>
+        <v>112</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E67" s="7">
         <v>-1</v>
@@ -5331,11 +5331,11 @@
       <c r="B68" s="7">
         <v>1</v>
       </c>
-      <c r="C68" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>93</v>
+      <c r="C68" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="E68" s="7">
         <v>2</v>
@@ -5361,20 +5361,20 @@
       <c r="L68" s="7">
         <v>2</v>
       </c>
-      <c r="M68" s="13" t="s">
-        <v>198</v>
+      <c r="M68" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N68" s="7">
         <v>3</v>
       </c>
-      <c r="O68" s="13" t="s">
-        <v>205</v>
+      <c r="O68" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="P68" s="7">
         <v>3</v>
       </c>
-      <c r="Q68" s="13" t="s">
-        <v>217</v>
+      <c r="Q68" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
@@ -5393,11 +5393,11 @@
       <c r="B69" s="7">
         <v>2</v>
       </c>
-      <c r="C69" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D69" s="13" t="s">
-        <v>94</v>
+      <c r="C69" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="E69" s="7">
         <v>6</v>
@@ -5423,20 +5423,20 @@
       <c r="L69" s="7">
         <v>1</v>
       </c>
-      <c r="M69" s="13" t="s">
-        <v>207</v>
+      <c r="M69" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="N69" s="7">
         <v>4</v>
       </c>
-      <c r="O69" s="13" t="s">
-        <v>205</v>
+      <c r="O69" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="P69" s="7">
         <v>2</v>
       </c>
-      <c r="Q69" s="13" t="s">
-        <v>209</v>
+      <c r="Q69" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="R69" s="2"/>
       <c r="S69" s="2"/>
@@ -5455,11 +5455,11 @@
       <c r="B70" s="7">
         <v>3</v>
       </c>
-      <c r="C70" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>95</v>
+      <c r="C70" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="E70" s="7">
         <v>7</v>
@@ -5485,8 +5485,8 @@
       <c r="L70" s="7">
         <v>2</v>
       </c>
-      <c r="M70" s="13" t="s">
-        <v>198</v>
+      <c r="M70" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N70" s="7">
         <v>-1</v>
@@ -5497,8 +5497,8 @@
       <c r="P70" s="7">
         <v>3</v>
       </c>
-      <c r="Q70" s="13" t="s">
-        <v>217</v>
+      <c r="Q70" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="R70" s="2"/>
       <c r="S70" s="2"/>
@@ -5517,11 +5517,11 @@
       <c r="B71" s="7">
         <v>4</v>
       </c>
-      <c r="C71" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>96</v>
+      <c r="C71" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="E71" s="7">
         <v>6</v>
@@ -5547,20 +5547,20 @@
       <c r="L71" s="7">
         <v>2</v>
       </c>
-      <c r="M71" s="13" t="s">
-        <v>198</v>
+      <c r="M71" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N71" s="7">
         <v>3</v>
       </c>
-      <c r="O71" s="13" t="s">
-        <v>205</v>
+      <c r="O71" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="P71" s="7">
         <v>2</v>
       </c>
-      <c r="Q71" s="13" t="s">
-        <v>209</v>
+      <c r="Q71" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="R71" s="2"/>
       <c r="S71" s="2"/>
@@ -5580,10 +5580,10 @@
         <v>5</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>97</v>
+        <v>112</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="E72" s="7">
         <v>-1</v>
@@ -5642,10 +5642,10 @@
         <v>6</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="E73" s="7">
         <v>-1</v>
@@ -5704,10 +5704,10 @@
         <v>7</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D74" s="13" t="s">
-        <v>99</v>
+        <v>112</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="E74" s="7">
         <v>-1</v>
@@ -5765,11 +5765,11 @@
       <c r="B75" s="7">
         <v>1</v>
       </c>
-      <c r="C75" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>100</v>
+      <c r="C75" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="E75" s="7">
         <v>2</v>
@@ -5795,20 +5795,20 @@
       <c r="L75" s="7">
         <v>2</v>
       </c>
-      <c r="M75" s="13" t="s">
-        <v>198</v>
+      <c r="M75" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N75" s="7">
         <v>3</v>
       </c>
-      <c r="O75" s="13" t="s">
-        <v>218</v>
+      <c r="O75" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="P75" s="7">
         <v>3</v>
       </c>
-      <c r="Q75" s="13" t="s">
-        <v>201</v>
+      <c r="Q75" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="R75" s="2"/>
       <c r="S75" s="2"/>
@@ -5827,11 +5827,11 @@
       <c r="B76" s="7">
         <v>2</v>
       </c>
-      <c r="C76" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>101</v>
+      <c r="C76" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="E76" s="7">
         <v>5</v>
@@ -5857,20 +5857,20 @@
       <c r="L76" s="7">
         <v>2</v>
       </c>
-      <c r="M76" s="13" t="s">
-        <v>198</v>
+      <c r="M76" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="N76" s="7">
         <v>3</v>
       </c>
-      <c r="O76" s="13" t="s">
-        <v>218</v>
+      <c r="O76" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="P76" s="7">
         <v>3</v>
       </c>
-      <c r="Q76" s="13" t="s">
-        <v>201</v>
+      <c r="Q76" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="R76" s="2"/>
       <c r="S76" s="2"/>
@@ -5889,11 +5889,11 @@
       <c r="B77" s="7">
         <v>3</v>
       </c>
-      <c r="C77" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="D77" s="13" t="s">
-        <v>102</v>
+      <c r="C77" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="E77" s="7">
         <v>2</v>
@@ -5919,8 +5919,8 @@
       <c r="L77" s="7">
         <v>3</v>
       </c>
-      <c r="M77" s="13" t="s">
-        <v>219</v>
+      <c r="M77" s="9" t="s">
+        <v>218</v>
       </c>
       <c r="N77" s="7">
         <v>-1</v>
@@ -5931,8 +5931,8 @@
       <c r="P77" s="7">
         <v>3</v>
       </c>
-      <c r="Q77" s="13" t="s">
-        <v>220</v>
+      <c r="Q77" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="R77" s="2"/>
       <c r="S77" s="2"/>
@@ -5951,11 +5951,11 @@
       <c r="B78" s="7">
         <v>4</v>
       </c>
-      <c r="C78" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>103</v>
+      <c r="C78" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="E78" s="7">
         <v>5</v>
@@ -5981,14 +5981,14 @@
       <c r="L78" s="7">
         <v>2</v>
       </c>
-      <c r="M78" s="13" t="s">
-        <v>221</v>
+      <c r="M78" s="9" t="s">
+        <v>220</v>
       </c>
       <c r="N78" s="7">
         <v>4</v>
       </c>
-      <c r="O78" s="13" t="s">
-        <v>222</v>
+      <c r="O78" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="P78" s="7">
         <v>-1</v>
@@ -6013,11 +6013,11 @@
       <c r="B79" s="7">
         <v>5</v>
       </c>
-      <c r="C79" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D79" s="13" t="s">
-        <v>104</v>
+      <c r="C79" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="E79" s="7">
         <v>7</v>
@@ -6043,14 +6043,14 @@
       <c r="L79" s="7">
         <v>1</v>
       </c>
-      <c r="M79" s="13" t="s">
-        <v>207</v>
+      <c r="M79" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="N79" s="7">
         <v>4</v>
       </c>
-      <c r="O79" s="13" t="s">
-        <v>222</v>
+      <c r="O79" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="P79" s="7">
         <v>-1</v>
@@ -6075,11 +6075,11 @@
       <c r="B80" s="7">
         <v>6</v>
       </c>
-      <c r="C80" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D80" s="13" t="s">
-        <v>105</v>
+      <c r="C80" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="E80" s="7">
         <v>8</v>
@@ -6105,8 +6105,8 @@
       <c r="L80" s="7">
         <v>3</v>
       </c>
-      <c r="M80" s="13" t="s">
-        <v>223</v>
+      <c r="M80" s="9" t="s">
+        <v>222</v>
       </c>
       <c r="N80" s="7">
         <v>-1</v>
@@ -6137,11 +6137,11 @@
       <c r="B81" s="7">
         <v>7</v>
       </c>
-      <c r="C81" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>106</v>
+      <c r="C81" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="E81" s="7">
         <v>9</v>
@@ -6167,8 +6167,8 @@
       <c r="L81" s="7">
         <v>3</v>
       </c>
-      <c r="M81" s="13" t="s">
-        <v>224</v>
+      <c r="M81" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="N81" s="7">
         <v>-1</v>
@@ -6200,10 +6200,10 @@
         <v>8</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D82" s="13" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="E82" s="7">
         <v>-1</v>
@@ -6262,10 +6262,10 @@
         <v>9</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="E83" s="7">
         <v>-1</v>

</xml_diff>